<commit_message>
fixed updating QTableWidget for recalculate function and show only 1 decimal place
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inspiron3650\Documents\PythonScripts\TrailCampPlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6F2D5A-ABFD-4A80-98C0-24579B28ED00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A7CD3F-10C7-4DD6-A468-2DC38789BB7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1C894634-F30C-4AA5-BD8B-F595E55EC65F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Lupine Meadows TH</t>
   </si>
@@ -69,12 +69,6 @@
     <t>Holly Lake</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>End</t>
-  </si>
-  <si>
     <t>Miles</t>
   </si>
   <si>
@@ -130,6 +124,9 @@
   </si>
   <si>
     <t>Garnet Canyon JCT</t>
+  </si>
+  <si>
+    <t>Site</t>
   </si>
 </sst>
 </file>
@@ -179,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -188,7 +185,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -517,295 +513,286 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E13037-8E4A-4ACD-8693-F32F25985FFD}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2">
+      <c r="B4" s="2">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="B5" s="2">
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2">
+      <c r="B6" s="2">
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2">
+      <c r="B7" s="2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="B8" s="2">
         <v>1.3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3" t="s">
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5">
+      <c r="B9" s="4">
         <v>1.3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="3" t="s">
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5">
+      <c r="B10" s="4">
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2">
+      <c r="B11" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2">
+      <c r="B12" s="2">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="2">
+      <c r="B13" s="2">
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="7">
+      <c r="B14" s="6">
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="7">
+      <c r="B17" s="6">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="6">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="6">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="9">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="9">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="6">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="6">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="6">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="6">
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="7">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="7">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="7">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="7">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="7">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="7">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="7">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="7">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="10">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="10">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="10">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="10">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="7">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="7">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="7">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="7">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="7">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="8" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="7">
+      <c r="B34" s="6">
         <v>1.7</v>
       </c>
     </row>

</xml_diff>